<commit_message>
Commit Brand code and wash day
</commit_message>
<xml_diff>
--- a/Upkeep_v3/Upkeep_v3/Cocktail_World/Template/Brand Code.xlsx
+++ b/Upkeep_v3/Upkeep_v3/Cocktail_World/Template/Brand Code.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ee5802a9bf16156/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh Araple\Source\Repos\Compel-admin\Upkeep_v3_Projects\Upkeep_v3\Upkeep_v3\Cocktail_World\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D278CDD0-1345-400B-B3C6-8CA3CD8818E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A7973C-07D9-4B72-ABB2-428150E9B7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E44C0104-A013-41CF-A052-D0D7F2CEE282}"/>
   </bookViews>
@@ -33,16 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Speg</t>
   </si>
@@ -50,7 +41,28 @@
     <t>Bottle</t>
   </si>
   <si>
-    <t>lPeg</t>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>spe</t>
+  </si>
+  <si>
+    <t>Brand Name</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Lpeg</t>
+  </si>
+  <si>
+    <t>btl</t>
+  </si>
+  <si>
+    <t>xabc</t>
+  </si>
+  <si>
+    <t>License Name</t>
   </si>
 </sst>
 </file>
@@ -412,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB14B85-1C92-434A-BEA8-F2DA3A838B02}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,22 +442,50 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>750</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="F3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>